<commit_message>
p_i value calculations added
</commit_message>
<xml_diff>
--- a/data/konut-fiyat-endeks.xlsx
+++ b/data/konut-fiyat-endeks.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="153">
   <si>
     <t>Tarih</t>
   </si>
@@ -473,57 +473,6 @@
   </si>
   <si>
     <t>2024-01</t>
-  </si>
-  <si>
-    <t>Seri Açıklamaları</t>
-  </si>
-  <si>
-    <t>TP.HKFE01</t>
-  </si>
-  <si>
-    <t>Konut Fiyat Endeksi (KFE)-Düzey</t>
-  </si>
-  <si>
-    <t>Gözlem Değeri: Bitiş</t>
-  </si>
-  <si>
-    <t>Notlar</t>
-  </si>
-  <si>
-    <t>Uygulama Değişiklik Linki</t>
-  </si>
-  <si>
-    <t>http://www.tcmb.gov.tr/wps/wcm/connect/TR/TCMB+TR/Main+Menu/Istatistikler/Reel+Sektor+Istatistikleri/Konut+Fiyat+Endeksi/Uygulama+Degisiklikleri</t>
-  </si>
-  <si>
-    <t>Veri Kaynağı</t>
-  </si>
-  <si>
-    <t>TCMB</t>
-  </si>
-  <si>
-    <t>Veri Yayınlama Takvim Linki</t>
-  </si>
-  <si>
-    <t>https://www3.tcmb.gov.tr/veriyaytakvim/takvim.php?yayim_id=11&amp;ay=99&amp;B1=ARA</t>
-  </si>
-  <si>
-    <t>Metaveri Linki</t>
-  </si>
-  <si>
-    <t>http://www.tcmb.gov.tr/wps/wcm/connect/TR/TCMB+TR/Main+Menu/Istatistikler/Reel+Sektor+Istatistikleri/Konut+Fiyat+Endeksi/Metaveri</t>
-  </si>
-  <si>
-    <t>Etiketler</t>
-  </si>
-  <si>
-    <t>Konut, Konut, Fiyatları, KFE, HKFE, Hedonik, Konut, Fiyat, Endeksi, Konut, Fiyat, Endeksi</t>
-  </si>
-  <si>
-    <t>Dipnotlar</t>
-  </si>
-  <si>
-    <t>Adıyaman, Malatya, Hatay, Kahramanmaraş ve Osmaniye illerinde depreme bağlı olarak veri sayısının yetersiz olması nedeniyle söz konusu illerde 2023 yılı Şubat ayından itibaren endeksler sabit kabul edilmiştir.</t>
   </si>
 </sst>
 </file>
@@ -531,7 +480,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -542,12 +491,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -579,7 +522,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -590,23 +533,14 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -910,18 +844,18 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C164"/>
+  <dimension ref="A1:C152"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -931,1459 +865,1363 @@
       <c r="C1" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>50</v>
       </c>
       <c r="C2" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>50</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>50.6</v>
       </c>
       <c r="C4" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>50.9</v>
       </c>
       <c r="C5" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>51.1</v>
       </c>
       <c r="C6" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>51.2</v>
       </c>
       <c r="C7" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <v>51.7</v>
       </c>
       <c r="C8" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="4">
         <v>52.5</v>
       </c>
       <c r="C9" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="4">
         <v>53</v>
       </c>
       <c r="C10" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="4">
         <v>53.6</v>
       </c>
       <c r="C11" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="4">
         <v>54.3</v>
       </c>
       <c r="C12" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="4">
         <v>54.7</v>
       </c>
       <c r="C13" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="4">
         <v>55.1</v>
       </c>
       <c r="C14" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="4">
         <v>55.4</v>
       </c>
       <c r="C15" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="4">
         <v>55.5</v>
       </c>
       <c r="C16" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="4">
         <v>55.7</v>
       </c>
       <c r="C17" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="4">
         <v>56</v>
       </c>
       <c r="C18" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="4">
         <v>56.4</v>
       </c>
       <c r="C19" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="4">
         <v>56.9</v>
       </c>
       <c r="C20" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="4">
         <v>57.6</v>
       </c>
       <c r="C21" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22" s="4">
         <v>58.4</v>
       </c>
       <c r="C22" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23" s="4">
         <v>59.2</v>
       </c>
       <c r="C23" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24" s="4">
         <v>60</v>
       </c>
       <c r="C24" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B25" s="4">
         <v>60.6</v>
       </c>
       <c r="C25" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26" s="4">
         <v>61.2</v>
       </c>
       <c r="C26" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="5">
+      <c r="B27" s="4">
         <v>61.5</v>
       </c>
       <c r="C27" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="5">
+      <c r="B28" s="4">
         <v>62</v>
       </c>
       <c r="C28" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="5">
+      <c r="B29" s="4">
         <v>62.5</v>
       </c>
       <c r="C29" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="5">
+      <c r="B30" s="4">
         <v>63.3</v>
       </c>
       <c r="C30" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="5">
+      <c r="B31" s="4">
         <v>63.6</v>
       </c>
       <c r="C31" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="5">
+      <c r="B32" s="4">
         <v>64.1</v>
       </c>
       <c r="C32" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="5">
+      <c r="B33" s="4">
         <v>64.8</v>
       </c>
       <c r="C33" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="5">
+      <c r="B34" s="4">
         <v>65.7</v>
       </c>
       <c r="C34" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="5">
+      <c r="B35" s="4">
         <v>66.8</v>
       </c>
       <c r="C35" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B36" s="5">
+      <c r="B36" s="4">
         <v>67.5</v>
       </c>
       <c r="C36" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B37" s="5">
+      <c r="B37" s="4">
         <v>68.2</v>
       </c>
       <c r="C37" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B38" s="5">
+      <c r="B38" s="4">
         <v>69.3</v>
       </c>
       <c r="C38" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
-      <c r="A39" s="4" t="s">
+      <c r="A39" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B39" s="5">
+      <c r="B39" s="4">
         <v>70.2</v>
       </c>
       <c r="C39" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
-      <c r="A40" s="4" t="s">
+      <c r="A40" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B40" s="5">
+      <c r="B40" s="4">
         <v>70.9</v>
       </c>
       <c r="C40" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
-      <c r="A41" s="4" t="s">
+      <c r="A41" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B41" s="5">
+      <c r="B41" s="4">
         <v>71.5</v>
       </c>
       <c r="C41" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B42" s="5">
+      <c r="B42" s="4">
         <v>72.4</v>
       </c>
       <c r="C42" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
-      <c r="A43" s="4" t="s">
+      <c r="A43" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B43" s="5">
+      <c r="B43" s="4">
         <v>73.1</v>
       </c>
       <c r="C43" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
-      <c r="A44" s="4" t="s">
+      <c r="A44" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B44" s="5">
+      <c r="B44" s="4">
         <v>74.2</v>
       </c>
       <c r="C44" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
-      <c r="A45" s="4" t="s">
+      <c r="A45" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B45" s="5">
+      <c r="B45" s="4">
         <v>75.4</v>
       </c>
       <c r="C45" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
-      <c r="A46" s="4" t="s">
+      <c r="A46" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B46" s="5">
+      <c r="B46" s="4">
         <v>76.6</v>
       </c>
       <c r="C46" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
-      <c r="A47" s="4" t="s">
+      <c r="A47" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B47" s="5">
+      <c r="B47" s="4">
         <v>77.7</v>
       </c>
       <c r="C47" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
-      <c r="A48" s="4" t="s">
+      <c r="A48" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B48" s="5">
+      <c r="B48" s="4">
         <v>78.9</v>
       </c>
       <c r="C48" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
-      <c r="A49" s="4" t="s">
+      <c r="A49" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B49" s="5">
+      <c r="B49" s="4">
         <v>79.9</v>
       </c>
       <c r="C49" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
-      <c r="A50" s="4" t="s">
+      <c r="A50" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B50" s="5">
+      <c r="B50" s="4">
         <v>80.6</v>
       </c>
       <c r="C50" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
-      <c r="A51" s="4" t="s">
+      <c r="A51" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B51" s="5">
+      <c r="B51" s="4">
         <v>81.1</v>
       </c>
       <c r="C51" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
-      <c r="A52" s="4" t="s">
+      <c r="A52" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B52" s="5">
+      <c r="B52" s="4">
         <v>81.7</v>
       </c>
       <c r="C52" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
-      <c r="A53" s="4" t="s">
+      <c r="A53" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B53" s="5">
+      <c r="B53" s="4">
         <v>82.7</v>
       </c>
       <c r="C53" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
-      <c r="A54" s="4" t="s">
+      <c r="A54" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B54" s="5">
+      <c r="B54" s="4">
         <v>83.7</v>
       </c>
       <c r="C54" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
-      <c r="A55" s="4" t="s">
+      <c r="A55" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B55" s="5">
+      <c r="B55" s="4">
         <v>84.5</v>
       </c>
       <c r="C55" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
-      <c r="A56" s="4" t="s">
+      <c r="A56" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B56" s="5">
+      <c r="B56" s="4">
         <v>85.7</v>
       </c>
       <c r="C56" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
-      <c r="A57" s="4" t="s">
+      <c r="A57" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B57" s="5">
+      <c r="B57" s="4">
         <v>86.6</v>
       </c>
       <c r="C57" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
-      <c r="A58" s="4" t="s">
+      <c r="A58" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B58" s="5">
+      <c r="B58" s="4">
         <v>87.5</v>
       </c>
       <c r="C58" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
-      <c r="A59" s="4" t="s">
+      <c r="A59" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B59" s="5">
+      <c r="B59" s="4">
         <v>88.6</v>
       </c>
       <c r="C59" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
-      <c r="A60" s="4" t="s">
+      <c r="A60" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B60" s="5">
+      <c r="B60" s="4">
         <v>89.7</v>
       </c>
       <c r="C60" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
-      <c r="A61" s="4" t="s">
+      <c r="A61" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B61" s="5">
+      <c r="B61" s="4">
         <v>90.5</v>
       </c>
       <c r="C61" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
-      <c r="A62" s="4" t="s">
+      <c r="A62" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B62" s="5">
+      <c r="B62" s="4">
         <v>91.3</v>
       </c>
       <c r="C62" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
-      <c r="A63" s="4" t="s">
+      <c r="A63" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B63" s="5">
+      <c r="B63" s="4">
         <v>92.3</v>
       </c>
       <c r="C63" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
-      <c r="A64" s="4" t="s">
+      <c r="A64" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B64" s="5">
+      <c r="B64" s="4">
         <v>92.8</v>
       </c>
       <c r="C64" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
-      <c r="A65" s="4" t="s">
+      <c r="A65" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B65" s="5">
+      <c r="B65" s="4">
         <v>93.5</v>
       </c>
       <c r="C65" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
-      <c r="A66" s="4" t="s">
+      <c r="A66" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B66" s="5">
+      <c r="B66" s="4">
         <v>94</v>
       </c>
       <c r="C66" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
-      <c r="A67" s="4" t="s">
+      <c r="A67" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B67" s="5">
+      <c r="B67" s="4">
         <v>94.8</v>
       </c>
       <c r="C67" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
-      <c r="A68" s="4" t="s">
+      <c r="A68" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B68" s="5">
+      <c r="B68" s="4">
         <v>95.5</v>
       </c>
       <c r="C68" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
-      <c r="A69" s="4" t="s">
+      <c r="A69" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B69" s="5">
+      <c r="B69" s="4">
         <v>96.7</v>
       </c>
       <c r="C69" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75">
-      <c r="A70" s="4" t="s">
+      <c r="A70" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B70" s="5">
+      <c r="B70" s="4">
         <v>97.9</v>
       </c>
       <c r="C70" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75">
-      <c r="A71" s="4" t="s">
+      <c r="A71" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B71" s="5">
+      <c r="B71" s="4">
         <v>98.7</v>
       </c>
       <c r="C71" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75">
-      <c r="A72" s="4" t="s">
+      <c r="A72" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B72" s="5">
+      <c r="B72" s="4">
         <v>99.8</v>
       </c>
       <c r="C72" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75">
-      <c r="A73" s="4" t="s">
+      <c r="A73" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B73" s="5">
+      <c r="B73" s="4">
         <v>100.3</v>
       </c>
       <c r="C73" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75">
-      <c r="A74" s="4" t="s">
+      <c r="A74" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B74" s="5">
+      <c r="B74" s="4">
         <v>100.5</v>
       </c>
       <c r="C74" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75">
-      <c r="A75" s="4" t="s">
+      <c r="A75" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B75" s="5">
+      <c r="B75" s="4">
         <v>100.8</v>
       </c>
       <c r="C75" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75">
-      <c r="A76" s="4" t="s">
+      <c r="A76" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B76" s="5">
+      <c r="B76" s="4">
         <v>101.4</v>
       </c>
       <c r="C76" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
-      <c r="A77" s="4" t="s">
+      <c r="A77" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B77" s="5">
+      <c r="B77" s="4">
         <v>102.2</v>
       </c>
       <c r="C77" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
-      <c r="A78" s="4" t="s">
+      <c r="A78" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B78" s="5">
+      <c r="B78" s="4">
         <v>102.8</v>
       </c>
       <c r="C78" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
-      <c r="A79" s="4" t="s">
+      <c r="A79" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B79" s="5">
+      <c r="B79" s="4">
         <v>103.4</v>
       </c>
       <c r="C79" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75">
-      <c r="A80" s="4" t="s">
+      <c r="A80" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B80" s="5">
+      <c r="B80" s="4">
         <v>104.1</v>
       </c>
       <c r="C80" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75">
-      <c r="A81" s="4" t="s">
+      <c r="A81" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B81" s="5">
+      <c r="B81" s="4">
         <v>104.8</v>
       </c>
       <c r="C81" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75">
-      <c r="A82" s="4" t="s">
+      <c r="A82" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B82" s="5">
+      <c r="B82" s="4">
         <v>105.7</v>
       </c>
       <c r="C82" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75">
-      <c r="A83" s="4" t="s">
+      <c r="A83" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B83" s="5">
+      <c r="B83" s="4">
         <v>107.1</v>
       </c>
       <c r="C83" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18.75">
-      <c r="A84" s="4" t="s">
+      <c r="A84" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B84" s="5">
+      <c r="B84" s="4">
         <v>108.6</v>
       </c>
       <c r="C84" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75">
-      <c r="A85" s="4" t="s">
+      <c r="A85" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B85" s="5">
+      <c r="B85" s="4">
         <v>109.1</v>
       </c>
       <c r="C85" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75">
-      <c r="A86" s="4" t="s">
+      <c r="A86" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B86" s="5">
+      <c r="B86" s="4">
         <v>109.3</v>
       </c>
       <c r="C86" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75">
-      <c r="A87" s="4" t="s">
+      <c r="A87" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B87" s="5">
+      <c r="B87" s="4">
         <v>108.7</v>
       </c>
       <c r="C87" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75">
-      <c r="A88" s="4" t="s">
+      <c r="A88" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B88" s="5">
+      <c r="B88" s="4">
         <v>107.8</v>
       </c>
       <c r="C88" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75">
-      <c r="A89" s="4" t="s">
+      <c r="A89" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B89" s="5">
+      <c r="B89" s="4">
         <v>108.5</v>
       </c>
       <c r="C89" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75">
-      <c r="A90" s="4" t="s">
+      <c r="A90" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B90" s="5">
+      <c r="B90" s="4">
         <v>109.2</v>
       </c>
       <c r="C90" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75">
-      <c r="A91" s="4" t="s">
+      <c r="A91" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B91" s="5">
+      <c r="B91" s="4">
         <v>108</v>
       </c>
       <c r="C91" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75">
-      <c r="A92" s="4" t="s">
+      <c r="A92" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B92" s="5">
+      <c r="B92" s="4">
         <v>107.6</v>
       </c>
       <c r="C92" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75">
-      <c r="A93" s="4" t="s">
+      <c r="A93" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B93" s="5">
+      <c r="B93" s="4">
         <v>108.6</v>
       </c>
       <c r="C93" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18.75">
-      <c r="A94" s="4" t="s">
+      <c r="A94" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B94" s="5">
+      <c r="B94" s="4">
         <v>109</v>
       </c>
       <c r="C94" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18.75">
-      <c r="A95" s="4" t="s">
+      <c r="A95" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B95" s="5">
+      <c r="B95" s="4">
         <v>109.3</v>
       </c>
       <c r="C95" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75">
-      <c r="A96" s="4" t="s">
+      <c r="A96" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B96" s="5">
+      <c r="B96" s="4">
         <v>110.2</v>
       </c>
       <c r="C96" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
-      <c r="A97" s="4" t="s">
+      <c r="A97" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B97" s="5">
+      <c r="B97" s="4">
         <v>111</v>
       </c>
       <c r="C97" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18.75">
-      <c r="A98" s="4" t="s">
+      <c r="A98" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B98" s="5">
+      <c r="B98" s="4">
         <v>112.4</v>
       </c>
       <c r="C98" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18.75">
-      <c r="A99" s="4" t="s">
+      <c r="A99" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B99" s="5">
+      <c r="B99" s="4">
         <v>114.4</v>
       </c>
       <c r="C99" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="18.75">
-      <c r="A100" s="4" t="s">
+      <c r="A100" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B100" s="5">
+      <c r="B100" s="4">
         <v>115.2</v>
       </c>
       <c r="C100" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="18.75">
-      <c r="A101" s="4" t="s">
+      <c r="A101" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B101" s="5">
+      <c r="B101" s="4">
         <v>116</v>
       </c>
       <c r="C101" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="18.75">
-      <c r="A102" s="4" t="s">
+      <c r="A102" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B102" s="5">
+      <c r="B102" s="4">
         <v>117.1</v>
       </c>
       <c r="C102" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="18.75">
-      <c r="A103" s="4" t="s">
+      <c r="A103" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B103" s="5">
+      <c r="B103" s="4">
         <v>118.8</v>
       </c>
       <c r="C103" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="18.75">
-      <c r="A104" s="4" t="s">
+      <c r="A104" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B104" s="5">
+      <c r="B104" s="4">
         <v>120.9</v>
       </c>
       <c r="C104" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="18.75">
-      <c r="A105" s="4" t="s">
+      <c r="A105" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B105" s="5">
+      <c r="B105" s="4">
         <v>123.7</v>
       </c>
       <c r="C105" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="18.75">
-      <c r="A106" s="4" t="s">
+      <c r="A106" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B106" s="5">
+      <c r="B106" s="4">
         <v>125.4</v>
       </c>
       <c r="C106" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="18.75">
-      <c r="A107" s="4" t="s">
+      <c r="A107" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B107" s="5">
+      <c r="B107" s="4">
         <v>127.5</v>
       </c>
       <c r="C107" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="18.75">
-      <c r="A108" s="4" t="s">
+      <c r="A108" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B108" s="5">
+      <c r="B108" s="4">
         <v>135.9</v>
       </c>
       <c r="C108" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="18.75">
-      <c r="A109" s="4" t="s">
+      <c r="A109" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B109" s="5">
+      <c r="B109" s="4">
         <v>139.5</v>
       </c>
       <c r="C109" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="18.75">
-      <c r="A110" s="4" t="s">
+      <c r="A110" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B110" s="5">
+      <c r="B110" s="4">
         <v>141.4</v>
       </c>
       <c r="C110" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="18.75">
-      <c r="A111" s="4" t="s">
+      <c r="A111" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B111" s="5">
+      <c r="B111" s="4">
         <v>144.4</v>
       </c>
       <c r="C111" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="18.75">
-      <c r="A112" s="4" t="s">
+      <c r="A112" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B112" s="5">
+      <c r="B112" s="4">
         <v>146.7</v>
       </c>
       <c r="C112" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="18.75">
-      <c r="A113" s="4" t="s">
+      <c r="A113" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B113" s="5">
+      <c r="B113" s="4">
         <v>149.9</v>
       </c>
       <c r="C113" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="18.75">
-      <c r="A114" s="4" t="s">
+      <c r="A114" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B114" s="5">
+      <c r="B114" s="4">
         <v>152.2</v>
       </c>
       <c r="C114" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="18.75">
-      <c r="A115" s="4" t="s">
+      <c r="A115" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B115" s="5">
+      <c r="B115" s="4">
         <v>154.9</v>
       </c>
       <c r="C115" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="18.75">
-      <c r="A116" s="4" t="s">
+      <c r="A116" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B116" s="5">
+      <c r="B116" s="4">
         <v>157.7</v>
       </c>
       <c r="C116" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="18.75">
-      <c r="A117" s="4" t="s">
+      <c r="A117" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B117" s="5">
+      <c r="B117" s="4">
         <v>161.7</v>
       </c>
       <c r="C117" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="18.75">
-      <c r="A118" s="4" t="s">
+      <c r="A118" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B118" s="5">
+      <c r="B118" s="4">
         <v>165.5</v>
       </c>
       <c r="C118" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="18.75">
-      <c r="A119" s="4" t="s">
+      <c r="A119" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B119" s="5">
+      <c r="B119" s="4">
         <v>168.8</v>
       </c>
       <c r="C119" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="18.75">
-      <c r="A120" s="4" t="s">
+      <c r="A120" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B120" s="5">
+      <c r="B120" s="4">
         <v>175.4</v>
       </c>
       <c r="C120" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="18.75">
-      <c r="A121" s="4" t="s">
+      <c r="A121" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B121" s="5">
+      <c r="B121" s="4">
         <v>180.3</v>
       </c>
       <c r="C121" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="18.75">
-      <c r="A122" s="4" t="s">
+      <c r="A122" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B122" s="5">
+      <c r="B122" s="4">
         <v>185.4</v>
       </c>
       <c r="C122" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="18.75">
-      <c r="A123" s="4" t="s">
+      <c r="A123" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B123" s="5">
+      <c r="B123" s="4">
         <v>192.7</v>
       </c>
       <c r="C123" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="18.75">
-      <c r="A124" s="4" t="s">
+      <c r="A124" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B124" s="5">
+      <c r="B124" s="4">
         <v>198.9</v>
       </c>
       <c r="C124" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="18.75">
-      <c r="A125" s="4" t="s">
+      <c r="A125" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B125" s="5">
+      <c r="B125" s="4">
         <v>210.2</v>
       </c>
       <c r="C125" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="126" customHeight="1" ht="18.75">
-      <c r="A126" s="4" t="s">
+      <c r="A126" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B126" s="5">
+      <c r="B126" s="4">
         <v>229.2</v>
       </c>
       <c r="C126" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="18.75">
-      <c r="A127" s="4" t="s">
+      <c r="A127" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B127" s="5">
+      <c r="B127" s="4">
         <v>247.4</v>
       </c>
       <c r="C127" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="18.75">
-      <c r="A128" s="4" t="s">
+      <c r="A128" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B128" s="5">
+      <c r="B128" s="4">
         <v>279.9</v>
       </c>
       <c r="C128" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="18.75">
-      <c r="A129" s="4" t="s">
+      <c r="A129" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B129" s="5">
+      <c r="B129" s="4">
         <v>318</v>
       </c>
       <c r="C129" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="130" customHeight="1" ht="18.75">
-      <c r="A130" s="4" t="s">
+      <c r="A130" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B130" s="5">
+      <c r="B130" s="4">
         <v>347.7</v>
       </c>
       <c r="C130" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="18.75">
-      <c r="A131" s="4" t="s">
+      <c r="A131" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B131" s="5">
+      <c r="B131" s="4">
         <v>383</v>
       </c>
       <c r="C131" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="132" customHeight="1" ht="18.75">
-      <c r="A132" s="4" t="s">
+      <c r="A132" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B132" s="5">
+      <c r="B132" s="4">
         <v>431.1</v>
       </c>
       <c r="C132" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="133" customHeight="1" ht="18.75">
-      <c r="A133" s="4" t="s">
+      <c r="A133" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B133" s="5">
+      <c r="B133" s="4">
         <v>470</v>
       </c>
       <c r="C133" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="134" customHeight="1" ht="18.75">
-      <c r="A134" s="4" t="s">
+      <c r="A134" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B134" s="5">
+      <c r="B134" s="4">
         <v>507.8</v>
       </c>
       <c r="C134" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="135" customHeight="1" ht="18.75">
-      <c r="A135" s="4" t="s">
+      <c r="A135" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B135" s="5">
+      <c r="B135" s="4">
         <v>548.2</v>
       </c>
       <c r="C135" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="136" customHeight="1" ht="18.75">
-      <c r="A136" s="4" t="s">
+      <c r="A136" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B136" s="5">
+      <c r="B136" s="4">
         <v>575</v>
       </c>
       <c r="C136" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="137" customHeight="1" ht="18.75">
-      <c r="A137" s="4" t="s">
+      <c r="A137" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B137" s="5">
+      <c r="B137" s="4">
         <v>605.8</v>
       </c>
       <c r="C137" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="138" customHeight="1" ht="18.75">
-      <c r="A138" s="4" t="s">
+      <c r="A138" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B138" s="5">
+      <c r="B138" s="4">
         <v>629.2</v>
       </c>
       <c r="C138" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="139" customHeight="1" ht="18.75">
-      <c r="A139" s="4" t="s">
+      <c r="A139" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B139" s="5">
+      <c r="B139" s="4">
         <v>662.7</v>
       </c>
       <c r="C139" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="140" customHeight="1" ht="18.75">
-      <c r="A140" s="4" t="s">
+      <c r="A140" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B140" s="5">
+      <c r="B140" s="4">
         <v>708.5</v>
       </c>
       <c r="C140" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="141" customHeight="1" ht="18.75">
-      <c r="A141" s="4" t="s">
+      <c r="A141" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B141" s="5">
+      <c r="B141" s="4">
         <v>768.1</v>
       </c>
       <c r="C141" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="142" customHeight="1" ht="18.75">
-      <c r="A142" s="4" t="s">
+      <c r="A142" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B142" s="5">
+      <c r="B142" s="4">
         <v>809.6</v>
       </c>
       <c r="C142" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="143" customHeight="1" ht="18.75">
-      <c r="A143" s="4" t="s">
+      <c r="A143" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B143" s="5">
+      <c r="B143" s="4">
         <v>847.4</v>
       </c>
       <c r="C143" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="144" customHeight="1" ht="18.75">
-      <c r="A144" s="4" t="s">
+      <c r="A144" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B144" s="5">
+      <c r="B144" s="4">
         <v>878</v>
       </c>
       <c r="C144" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="145" customHeight="1" ht="18.75">
-      <c r="A145" s="4" t="s">
+      <c r="A145" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B145" s="5">
+      <c r="B145" s="4">
         <v>921</v>
       </c>
       <c r="C145" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="146" customHeight="1" ht="18.75">
-      <c r="A146" s="4" t="s">
+      <c r="A146" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B146" s="5">
+      <c r="B146" s="4">
         <v>988.7</v>
       </c>
       <c r="C146" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="147" customHeight="1" ht="18.75">
-      <c r="A147" s="4" t="s">
+      <c r="A147" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B147" s="5">
+      <c r="B147" s="4">
         <v>1043.1</v>
       </c>
       <c r="C147" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="148" customHeight="1" ht="18.75">
-      <c r="A148" s="4" t="s">
+      <c r="A148" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B148" s="5">
+      <c r="B148" s="4">
         <v>1087.9</v>
       </c>
       <c r="C148" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="149" customHeight="1" ht="18.75">
-      <c r="A149" s="4" t="s">
+      <c r="A149" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B149" s="5">
+      <c r="B149" s="4">
         <v>1129.5</v>
       </c>
       <c r="C149" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="150" customHeight="1" ht="18.75">
-      <c r="A150" s="4" t="s">
+      <c r="A150" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B150" s="5">
+      <c r="B150" s="4">
         <v>1150</v>
       </c>
       <c r="C150" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="151" customHeight="1" ht="18.75">
-      <c r="A151" s="4" t="s">
+      <c r="A151" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B151" s="5">
+      <c r="B151" s="4">
         <v>1163.3</v>
       </c>
       <c r="C151" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="152" customHeight="1" ht="18.75">
-      <c r="A152" s="4" t="s">
+      <c r="A152" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B152" s="5">
+      <c r="B152" s="4">
         <v>1190</v>
       </c>
       <c r="C152" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="18.75">
-      <c r="A153" s="3"/>
-      <c r="B153" s="6"/>
-      <c r="C153" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="154" customHeight="1" ht="18.75">
-      <c r="A154" s="3"/>
-      <c r="B154" s="6"/>
-      <c r="C154" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="155" customHeight="1" ht="18.75">
-      <c r="A155" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="B155" s="6"/>
-      <c r="C155" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="156" customHeight="1" ht="18.75">
-      <c r="A156" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="B156" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="C156" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="157" customHeight="1" ht="18.75">
-      <c r="A157" s="3"/>
-      <c r="B157" s="6"/>
-      <c r="C157" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="158" customHeight="1" ht="18.75">
-      <c r="A158" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="B158" s="6"/>
-      <c r="C158" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="159" customHeight="1" ht="18.75">
-      <c r="A159" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="B159" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C159" s="4" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="160" customHeight="1" ht="18.75">
-      <c r="A160" s="3"/>
-      <c r="B160" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="C160" s="4" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="161" customHeight="1" ht="18.75">
-      <c r="A161" s="3"/>
-      <c r="B161" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="C161" s="4" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="162" customHeight="1" ht="18.75">
-      <c r="A162" s="3"/>
-      <c r="B162" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="C162" s="4" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="163" customHeight="1" ht="18.75">
-      <c r="A163" s="3"/>
-      <c r="B163" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="C163" s="4" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="164" customHeight="1" ht="18.75">
-      <c r="A164" s="3"/>
-      <c r="B164" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="C164" s="3" t="s">
-        <v>169</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>